<commit_message>
badania stat do hipotez
</commit_message>
<xml_diff>
--- a/import_csv_02_legenda.xlsx
+++ b/import_csv_02_legenda.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robert/Work/PracaMagPiel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E59A8EC7-F0BE-2245-832E-0D021A9CE558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D29085-3DB4-1F49-B125-FAED09FD961C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2000" windowWidth="27640" windowHeight="16940" xr2:uid="{813AB0CC-C33C-1843-BA40-2F5F3753C7B6}"/>
+    <workbookView xWindow="17260" yWindow="-19420" windowWidth="39180" windowHeight="17640" xr2:uid="{813AB0CC-C33C-1843-BA40-2F5F3753C7B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4386" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4472" uniqueCount="219">
   <si>
     <t>Wiek</t>
   </si>
@@ -1112,10 +1112,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF557F92-D361-A143-8EB6-7F38A83D0626}">
-  <dimension ref="A1:AQ117"/>
+  <dimension ref="A1:AU117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO1" workbookViewId="0">
-      <selection activeCell="AQ1" sqref="A1:AQ1"/>
+    <sheetView tabSelected="1" topLeftCell="AP9" workbookViewId="0">
+      <selection activeCell="AT27" sqref="AT27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1157,9 +1157,10 @@
     <col min="41" max="41" width="42.83203125" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="51.5" customWidth="1"/>
     <col min="43" max="43" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="47" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>92</v>
       </c>
@@ -1289,8 +1290,14 @@
       <c r="AQ1" t="s">
         <v>218</v>
       </c>
+      <c r="AT1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>173</v>
+      </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>173</v>
       </c>
@@ -1420,8 +1427,14 @@
       <c r="AQ2" t="s">
         <v>172</v>
       </c>
+      <c r="AT2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>93</v>
       </c>
@@ -1551,8 +1564,14 @@
       <c r="AQ3" s="2" t="s">
         <v>140</v>
       </c>
+      <c r="AT3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>174</v>
+      </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>94</v>
       </c>
@@ -1682,8 +1701,14 @@
       <c r="AQ4" s="2" t="s">
         <v>150</v>
       </c>
+      <c r="AT4" t="s">
+        <v>176</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>177</v>
+      </c>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
         <v>99</v>
@@ -1811,8 +1836,14 @@
       <c r="AQ5" s="2" t="s">
         <v>141</v>
       </c>
+      <c r="AT5" t="s">
+        <v>106</v>
+      </c>
+      <c r="AU5" t="s">
+        <v>175</v>
+      </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
         <v>95</v>
@@ -1928,8 +1959,14 @@
       <c r="AQ6" s="2" t="s">
         <v>142</v>
       </c>
+      <c r="AT6" t="s">
+        <v>112</v>
+      </c>
+      <c r="AU6" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
         <v>98</v>
@@ -2039,8 +2076,14 @@
       <c r="AQ7" s="2" t="s">
         <v>143</v>
       </c>
+      <c r="AT7" t="s">
+        <v>118</v>
+      </c>
+      <c r="AU7" t="s">
+        <v>118</v>
+      </c>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="D8" t="s">
         <v>183</v>
@@ -2141,14 +2184,26 @@
       <c r="AQ8" s="2" t="s">
         <v>144</v>
       </c>
+      <c r="AT8" t="s">
+        <v>124</v>
+      </c>
+      <c r="AU8" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="AJ9" s="2"/>
       <c r="AK9" s="2"/>
       <c r="AL9" s="2"/>
+      <c r="AT9" t="s">
+        <v>128</v>
+      </c>
+      <c r="AU9" t="s">
+        <v>128</v>
+      </c>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="AG10" t="s">
         <v>159</v>
@@ -2156,8 +2211,14 @@
       <c r="AJ10" s="2"/>
       <c r="AK10" s="2"/>
       <c r="AL10" s="2"/>
+      <c r="AT10" t="s">
+        <v>135</v>
+      </c>
+      <c r="AU10" t="s">
+        <v>135</v>
+      </c>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="AG11" t="s">
         <v>160</v>
@@ -2165,50 +2226,98 @@
       <c r="AJ11" s="2"/>
       <c r="AK11" s="2"/>
       <c r="AL11" s="2"/>
+      <c r="AT11" t="s">
+        <v>186</v>
+      </c>
+      <c r="AU11" t="s">
+        <v>139</v>
+      </c>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="AJ12" s="2"/>
       <c r="AK12" s="2"/>
       <c r="AL12" s="2"/>
+      <c r="AT12" t="s">
+        <v>187</v>
+      </c>
+      <c r="AU12" t="s">
+        <v>152</v>
+      </c>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="AJ13" s="2"/>
       <c r="AK13" s="2"/>
       <c r="AL13" s="2"/>
+      <c r="AT13" t="s">
+        <v>188</v>
+      </c>
+      <c r="AU13" t="s">
+        <v>153</v>
+      </c>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="AJ14" s="2"/>
       <c r="AK14" s="2"/>
       <c r="AL14" s="2"/>
+      <c r="AT14" t="s">
+        <v>189</v>
+      </c>
+      <c r="AU14" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="AJ15" s="2"/>
       <c r="AK15" s="2"/>
       <c r="AL15" s="2"/>
+      <c r="AT15" t="s">
+        <v>190</v>
+      </c>
+      <c r="AU15" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="AJ16" s="2"/>
       <c r="AK16" s="2"/>
       <c r="AL16" s="2"/>
+      <c r="AT16" t="s">
+        <v>191</v>
+      </c>
+      <c r="AU16" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="AJ17" s="2"/>
       <c r="AK17" s="2"/>
       <c r="AL17" s="2"/>
+      <c r="AT17" t="s">
+        <v>192</v>
+      </c>
+      <c r="AU17" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="AJ18" s="2"/>
       <c r="AK18" s="2"/>
       <c r="AL18" s="2"/>
+      <c r="AT18" t="s">
+        <v>193</v>
+      </c>
+      <c r="AU18" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="N19" t="s">
         <v>61</v>
@@ -2273,8 +2382,14 @@
       <c r="AJ19" t="s">
         <v>38</v>
       </c>
+      <c r="AT19" t="s">
+        <v>194</v>
+      </c>
+      <c r="AU19" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="N20" t="s">
         <v>37</v>
@@ -2345,8 +2460,14 @@
       <c r="AJ20" t="s">
         <v>36</v>
       </c>
+      <c r="AT20" t="s">
+        <v>195</v>
+      </c>
+      <c r="AU20" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="N21" t="s">
         <v>51</v>
@@ -2417,8 +2538,14 @@
       <c r="AJ21" t="s">
         <v>34</v>
       </c>
+      <c r="AT21" t="s">
+        <v>196</v>
+      </c>
+      <c r="AU21" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="N22" t="s">
         <v>61</v>
@@ -2489,8 +2616,14 @@
       <c r="AJ22" t="s">
         <v>36</v>
       </c>
+      <c r="AT22" t="s">
+        <v>197</v>
+      </c>
+      <c r="AU22" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="23" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="N23" t="s">
         <v>36</v>
@@ -2561,8 +2694,14 @@
       <c r="AJ23" t="s">
         <v>34</v>
       </c>
+      <c r="AT23" t="s">
+        <v>198</v>
+      </c>
+      <c r="AU23" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="24" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="N24" t="s">
         <v>61</v>
@@ -2639,8 +2778,14 @@
       <c r="AL24" t="s">
         <v>36</v>
       </c>
+      <c r="AT24" t="s">
+        <v>199</v>
+      </c>
+      <c r="AU24" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="25" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="N25" t="s">
         <v>36</v>
@@ -2717,8 +2862,14 @@
       <c r="AL25" t="s">
         <v>36</v>
       </c>
+      <c r="AT25" t="s">
+        <v>200</v>
+      </c>
+      <c r="AU25" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="26" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="N26" t="s">
         <v>51</v>
@@ -2807,8 +2958,14 @@
       <c r="AQ26" t="s">
         <v>36</v>
       </c>
+      <c r="AT26" t="s">
+        <v>201</v>
+      </c>
+      <c r="AU26" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="27" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="N27" t="s">
         <v>36</v>
@@ -2897,8 +3054,14 @@
       <c r="AQ27" t="s">
         <v>37</v>
       </c>
+      <c r="AT27" t="s">
+        <v>202</v>
+      </c>
+      <c r="AU27" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="28" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="N28" t="s">
         <v>61</v>
@@ -2990,8 +3153,14 @@
       <c r="AQ28" t="s">
         <v>34</v>
       </c>
+      <c r="AT28" t="s">
+        <v>203</v>
+      </c>
+      <c r="AU28" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="29" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="N29" t="s">
         <v>61</v>
@@ -3083,8 +3252,14 @@
       <c r="AQ29" t="s">
         <v>38</v>
       </c>
+      <c r="AT29" t="s">
+        <v>204</v>
+      </c>
+      <c r="AU29" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="30" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>24</v>
       </c>
@@ -3214,8 +3389,14 @@
       <c r="AQ30" t="s">
         <v>36</v>
       </c>
+      <c r="AT30" t="s">
+        <v>205</v>
+      </c>
+      <c r="AU30" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="31" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>24</v>
       </c>
@@ -3345,8 +3526,14 @@
       <c r="AQ31" t="s">
         <v>36</v>
       </c>
+      <c r="AT31" t="s">
+        <v>206</v>
+      </c>
+      <c r="AU31" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="32" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>24</v>
       </c>
@@ -3476,8 +3663,14 @@
       <c r="AQ32" t="s">
         <v>36</v>
       </c>
+      <c r="AT32" t="s">
+        <v>207</v>
+      </c>
+      <c r="AU32" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="33" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>42</v>
       </c>
@@ -3607,8 +3800,14 @@
       <c r="AQ33" t="s">
         <v>36</v>
       </c>
+      <c r="AT33" t="s">
+        <v>208</v>
+      </c>
+      <c r="AU33" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="34" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>24</v>
       </c>
@@ -3738,8 +3937,14 @@
       <c r="AQ34" t="s">
         <v>34</v>
       </c>
+      <c r="AT34" t="s">
+        <v>209</v>
+      </c>
+      <c r="AU34" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="35" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>24</v>
       </c>
@@ -3869,8 +4074,14 @@
       <c r="AQ35" t="s">
         <v>37</v>
       </c>
+      <c r="AT35" t="s">
+        <v>210</v>
+      </c>
+      <c r="AU35" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="36" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>24</v>
       </c>
@@ -4000,8 +4211,14 @@
       <c r="AQ36" t="s">
         <v>36</v>
       </c>
+      <c r="AT36" t="s">
+        <v>211</v>
+      </c>
+      <c r="AU36" t="s">
+        <v>161</v>
+      </c>
     </row>
-    <row r="37" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>24</v>
       </c>
@@ -4131,8 +4348,14 @@
       <c r="AQ37" t="s">
         <v>51</v>
       </c>
+      <c r="AT37" t="s">
+        <v>212</v>
+      </c>
+      <c r="AU37" t="s">
+        <v>162</v>
+      </c>
     </row>
-    <row r="38" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>24</v>
       </c>
@@ -4262,8 +4485,14 @@
       <c r="AQ38" t="s">
         <v>36</v>
       </c>
+      <c r="AT38" t="s">
+        <v>213</v>
+      </c>
+      <c r="AU38" t="s">
+        <v>163</v>
+      </c>
     </row>
-    <row r="39" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>24</v>
       </c>
@@ -4393,8 +4622,14 @@
       <c r="AQ39" t="s">
         <v>36</v>
       </c>
+      <c r="AT39" t="s">
+        <v>214</v>
+      </c>
+      <c r="AU39" t="s">
+        <v>164</v>
+      </c>
     </row>
-    <row r="40" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>24</v>
       </c>
@@ -4524,8 +4759,14 @@
       <c r="AQ40" t="s">
         <v>36</v>
       </c>
+      <c r="AT40" t="s">
+        <v>215</v>
+      </c>
+      <c r="AU40" t="s">
+        <v>169</v>
+      </c>
     </row>
-    <row r="41" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>24</v>
       </c>
@@ -4655,8 +4896,14 @@
       <c r="AQ41" t="s">
         <v>51</v>
       </c>
+      <c r="AT41" t="s">
+        <v>216</v>
+      </c>
+      <c r="AU41" t="s">
+        <v>170</v>
+      </c>
     </row>
-    <row r="42" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>24</v>
       </c>
@@ -4786,8 +5033,14 @@
       <c r="AQ42" t="s">
         <v>36</v>
       </c>
+      <c r="AT42" t="s">
+        <v>217</v>
+      </c>
+      <c r="AU42" t="s">
+        <v>171</v>
+      </c>
     </row>
-    <row r="43" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>24</v>
       </c>
@@ -4917,8 +5170,14 @@
       <c r="AQ43" t="s">
         <v>38</v>
       </c>
+      <c r="AT43" t="s">
+        <v>218</v>
+      </c>
+      <c r="AU43" t="s">
+        <v>172</v>
+      </c>
     </row>
-    <row r="44" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>24</v>
       </c>
@@ -5049,7 +5308,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>24</v>
       </c>
@@ -5180,7 +5439,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>24</v>
       </c>
@@ -5311,7 +5570,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="47" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>24</v>
       </c>
@@ -5442,7 +5701,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>24</v>
       </c>

</xml_diff>